<commit_message>
Added recommendations/comments to risk list
</commit_message>
<xml_diff>
--- a/Documentation/Risk_List_FIRST_DRAFT.xlsx
+++ b/Documentation/Risk_List_FIRST_DRAFT.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\brdsb\Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44D4F7F4-AC20-4994-8E89-99F74401B15D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="3" r:id="rId1"/>
@@ -25,11 +19,11 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Risk_Tracking_Log!$B$6:$D$6</definedName>
     <definedName name="as">[1]DropDown_Elements!$A$2:$A$30</definedName>
     <definedName name="OLE_LINK1" localSheetId="1">Risk_Tracking_Log!#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">Risk_Tracking_Log!$A$1:$M$34</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">Risk_Tracking_Log!$A$1:$M$33</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">Risk_Tracking_Log!$1:$6</definedName>
     <definedName name="Risk_Area">DropDown_Elements!$A$2:$A$30</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -41,13 +35,13 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>eze3</author>
     <author>e</author>
   </authors>
   <commentList>
-    <comment ref="A6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000001000000}">
+    <comment ref="A6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -70,7 +64,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000002000000}">
+    <comment ref="B6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -132,7 +126,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000003000000}">
+    <comment ref="C6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -215,7 +209,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000004000000}">
+    <comment ref="D6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -297,7 +291,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E6" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000005000000}">
+    <comment ref="E6" authorId="1">
       <text>
         <r>
           <rPr>
@@ -380,7 +374,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000006000000}">
+    <comment ref="F6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -403,7 +397,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G6" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000007000000}">
+    <comment ref="G6" authorId="1">
       <text>
         <r>
           <rPr>
@@ -425,7 +419,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-000008000000}">
+    <comment ref="H6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -447,7 +441,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I6" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-000009000000}">
+    <comment ref="I6" authorId="1">
       <text>
         <r>
           <rPr>
@@ -469,7 +463,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J6" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000A000000}">
+    <comment ref="J6" authorId="1">
       <text>
         <r>
           <rPr>
@@ -491,7 +485,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K6" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000B000000}">
+    <comment ref="K6" authorId="1">
       <text>
         <r>
           <rPr>
@@ -513,7 +507,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L6" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000C000000}">
+    <comment ref="L6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -536,7 +530,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M6" authorId="1" shapeId="0" xr:uid="{00000000-0006-0000-0100-00000D000000}">
+    <comment ref="M6" authorId="1">
       <text>
         <r>
           <rPr>
@@ -563,7 +557,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="193">
   <si>
     <t>ID</t>
   </si>
@@ -579,9 +573,6 @@
   <si>
     <t>Current
 Status</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> &lt;optional&gt;</t>
   </si>
   <si>
     <t>&lt;required&gt;</t>
@@ -1274,12 +1265,6 @@
     <t>Team member advises the other members of the team that they are leaving the project.</t>
   </si>
   <si>
-    <t>Plan work items and milestones so that each team member is capable of taking up additional work if this scenario does occur. Ensure that work done is understandable by all other team members to allow them to pick up where others left off.</t>
-  </si>
-  <si>
-    <t>Team must be able to adapt work plans and milestones to account for changes in team structure.</t>
-  </si>
-  <si>
     <t>This would mean that the final product delivered to the project sponsor does not meet their standards or requirements, and is therefore rejected after completion of the majority of project work. This would mean that the project has failed at some point to meet or to adequetly identify project requirements and specifications.</t>
   </si>
   <si>
@@ -1294,12 +1279,6 @@
     <t>Project sponsor informs the team after delivery of the final product that it does not meet their expectations.</t>
   </si>
   <si>
-    <t>Ensure communication with the sponsor to ensure that the project requirements are understood and that expectations for the final product are understood.</t>
-  </si>
-  <si>
-    <t>Ensure that product and associated documentation is produced that meets assessment requirements to fulfil the assessment component of this project.</t>
-  </si>
-  <si>
     <t>If the final project creates a risk for the sponsor by failing to protect user security then it may be rejected by the sponsor or considered a failure in general due to the importance of this requirement.</t>
   </si>
   <si>
@@ -1445,16 +1424,116 @@
   </si>
   <si>
     <t>Ensure that backups are available either through the hosting service or through team members manually preparing backups of version control.</t>
+  </si>
+  <si>
+    <t>Resource Manager</t>
+  </si>
+  <si>
+    <t>Team Managed Project</t>
+  </si>
+  <si>
+    <t>A tool which can assist a workteam with resource allocation among projects</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>11</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ensure communication with the sponsor to ensure that the project requirements are understood and that expectations for the final product are understood. </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Ensure that product and associated documentation is produced that meets assessment requirements to fulfil the assessment component of this project. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>As well as gaining feedback iteratively from the sponsor to ensure that their requirements are being met</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan work items and milestones so that each team member is capable of taking up additional work if this scenario does occur. Ensure that work done is understandable by all other team members to allow them to pick up where others left off. </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Team must be able to adapt work plans and milestones to account for changes in team structure. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>or reduce scope in negotiation with the sponsor where possible to deliver a minimum viable product</t>
+    </r>
+  </si>
+  <si>
+    <t>Chosen technology stack has a too high cost to implement when standing up final product</t>
+  </si>
+  <si>
+    <t>Project team willl be required to invest their own money</t>
+  </si>
+  <si>
+    <t>Free hosted solutions are not viable</t>
+  </si>
+  <si>
+    <t>Hosting service does not meet performance requirement</t>
+  </si>
+  <si>
+    <t>ensure that one of the free technologies will meet the needs of the project</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Investigate free hosting solutions early  </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1544,6 +1623,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -2046,7 +2131,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2201,9 +2286,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -2305,6 +2387,36 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2769,14 +2881,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2791,168 +2903,168 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="87" t="str">
+      <c r="A1" s="86" t="str">
         <f>Risk_Tracking_Log!A1</f>
         <v>RISK MANAGEMENT LOG</v>
       </c>
-      <c r="B1" s="88"/>
+      <c r="B1" s="87"/>
     </row>
     <row r="2" spans="1:2" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="78" t="s">
-        <v>14</v>
+      <c r="A2" s="77" t="s">
+        <v>13</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="23"/>
       <c r="B3" s="16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="20"/>
       <c r="B4" s="17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="51" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.2">
       <c r="A6" s="21" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B6" s="51" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="67.5" x14ac:dyDescent="0.2">
       <c r="A7" s="21" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="51" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A8" s="21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" s="52" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A9" s="21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="51" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B10" s="51" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11" s="51" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B12" s="51" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A13" s="21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B13" s="51" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B14" s="51" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="21" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B15" s="51" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A16" s="21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B16" s="51" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="12" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="70" t="s">
-        <v>72</v>
-      </c>
-      <c r="B17" s="71" t="s">
-        <v>62</v>
+      <c r="A17" s="69" t="s">
+        <v>71</v>
+      </c>
+      <c r="B17" s="70" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="12" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="20" spans="1:2" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="34.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B21" s="24" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="12" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="24" spans="1:2" ht="12" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:2" ht="57" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="26" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B25" s="24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -2968,11 +3080,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:U34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" workbookViewId="0">
-      <selection activeCell="M22" sqref="M22"/>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2994,7 +3106,7 @@
   <sheetData>
     <row r="1" spans="1:21" s="7" customFormat="1" ht="18.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
@@ -3004,7 +3116,7 @@
       <c r="G1" s="29"/>
       <c r="H1" s="29"/>
       <c r="I1" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J1" s="30"/>
       <c r="K1" s="30"/>
@@ -3013,12 +3125,12 @@
     </row>
     <row r="2" spans="1:21" s="1" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2" s="31"/>
       <c r="C2" s="31"/>
-      <c r="D2" s="32" t="s">
-        <v>5</v>
+      <c r="D2" s="88" t="s">
+        <v>167</v>
       </c>
       <c r="E2" s="34"/>
       <c r="F2" s="33"/>
@@ -3030,28 +3142,28 @@
       </c>
       <c r="J2" s="32" t="str">
         <f>D2</f>
-        <v xml:space="preserve"> &lt;optional&gt;</v>
+        <v>Resource Manager</v>
       </c>
       <c r="K2" s="38"/>
-      <c r="L2" s="69"/>
-      <c r="M2" s="69"/>
-      <c r="N2" s="69"/>
-      <c r="O2" s="69"/>
-      <c r="P2" s="69"/>
-      <c r="Q2" s="69"/>
-      <c r="R2" s="69"/>
-      <c r="S2" s="69"/>
-      <c r="T2" s="69"/>
-      <c r="U2" s="69"/>
+      <c r="L2" s="68"/>
+      <c r="M2" s="68"/>
+      <c r="N2" s="68"/>
+      <c r="O2" s="68"/>
+      <c r="P2" s="68"/>
+      <c r="Q2" s="68"/>
+      <c r="R2" s="68"/>
+      <c r="S2" s="68"/>
+      <c r="T2" s="68"/>
+      <c r="U2" s="68"/>
     </row>
     <row r="3" spans="1:21" s="1" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B3" s="35"/>
       <c r="C3" s="35"/>
       <c r="D3" s="36" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E3" s="38"/>
       <c r="F3" s="37"/>
@@ -3066,25 +3178,25 @@
         <v>&lt;required&gt;</v>
       </c>
       <c r="K3" s="38"/>
-      <c r="L3" s="69"/>
-      <c r="M3" s="69"/>
-      <c r="N3" s="69"/>
-      <c r="O3" s="69"/>
-      <c r="P3" s="69"/>
-      <c r="Q3" s="69"/>
-      <c r="R3" s="69"/>
-      <c r="S3" s="69"/>
-      <c r="T3" s="69"/>
-      <c r="U3" s="69"/>
-    </row>
-    <row r="4" spans="1:21" s="1" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L3" s="68"/>
+      <c r="M3" s="68"/>
+      <c r="N3" s="68"/>
+      <c r="O3" s="68"/>
+      <c r="P3" s="68"/>
+      <c r="Q3" s="68"/>
+      <c r="R3" s="68"/>
+      <c r="S3" s="68"/>
+      <c r="T3" s="68"/>
+      <c r="U3" s="68"/>
+    </row>
+    <row r="4" spans="1:21" s="1" customFormat="1" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="35"/>
       <c r="C4" s="35"/>
-      <c r="D4" s="39" t="s">
-        <v>6</v>
+      <c r="D4" s="89" t="s">
+        <v>168</v>
       </c>
       <c r="E4" s="38"/>
       <c r="F4" s="37"/>
@@ -3096,98 +3208,98 @@
       </c>
       <c r="J4" s="39" t="str">
         <f>D4</f>
-        <v>&lt;required&gt;</v>
+        <v>Team Managed Project</v>
       </c>
       <c r="K4" s="38"/>
-      <c r="L4" s="69"/>
-      <c r="M4" s="69"/>
-      <c r="N4" s="69"/>
-      <c r="O4" s="69"/>
-      <c r="P4" s="69"/>
-      <c r="Q4" s="69"/>
-      <c r="R4" s="69"/>
-      <c r="S4" s="69"/>
-      <c r="T4" s="69"/>
-      <c r="U4" s="69"/>
-    </row>
-    <row r="5" spans="1:21" s="1" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="L4" s="68"/>
+      <c r="M4" s="68"/>
+      <c r="N4" s="68"/>
+      <c r="O4" s="68"/>
+      <c r="P4" s="68"/>
+      <c r="Q4" s="68"/>
+      <c r="R4" s="68"/>
+      <c r="S4" s="68"/>
+      <c r="T4" s="68"/>
+      <c r="U4" s="68"/>
+    </row>
+    <row r="5" spans="1:21" s="1" customFormat="1" ht="57" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" s="31"/>
       <c r="C5" s="40"/>
-      <c r="D5" s="53" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54"/>
-      <c r="G5" s="54"/>
-      <c r="H5" s="54"/>
+      <c r="D5" s="90" t="s">
+        <v>169</v>
+      </c>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
       <c r="I5" s="9" t="str">
         <f>A5</f>
         <v>Project Description:</v>
       </c>
-      <c r="J5" s="77" t="str">
+      <c r="J5" s="76" t="str">
         <f>D5</f>
-        <v>&lt;required&gt;</v>
-      </c>
-      <c r="K5" s="54"/>
-      <c r="L5" s="54"/>
-      <c r="M5" s="55"/>
-      <c r="N5" s="69"/>
-      <c r="O5" s="69"/>
-      <c r="P5" s="69"/>
-      <c r="Q5" s="69"/>
-      <c r="R5" s="69"/>
-      <c r="S5" s="69"/>
-      <c r="T5" s="69"/>
-      <c r="U5" s="69"/>
-    </row>
-    <row r="6" spans="1:21" s="3" customFormat="1" ht="34.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="57" t="s">
+        <v>A tool which can assist a workteam with resource allocation among projects</v>
+      </c>
+      <c r="K5" s="53"/>
+      <c r="L5" s="53"/>
+      <c r="M5" s="54"/>
+      <c r="N5" s="68"/>
+      <c r="O5" s="68"/>
+      <c r="P5" s="68"/>
+      <c r="Q5" s="68"/>
+      <c r="R5" s="68"/>
+      <c r="S5" s="68"/>
+      <c r="T5" s="68"/>
+      <c r="U5" s="68"/>
+    </row>
+    <row r="6" spans="1:21" s="3" customFormat="1" ht="23.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="56" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="58" t="s">
+      <c r="B6" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="58" t="s">
+      <c r="C6" s="57" t="s">
+        <v>55</v>
+      </c>
+      <c r="D6" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="D6" s="56" t="s">
+      <c r="E6" s="55" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" s="57" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="E6" s="56" t="s">
-        <v>55</v>
-      </c>
-      <c r="F6" s="58" t="s">
+      <c r="H6" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="58" t="s">
-        <v>58</v>
-      </c>
-      <c r="H6" s="61" t="s">
-        <v>27</v>
-      </c>
-      <c r="I6" s="56" t="s">
+      <c r="I6" s="55" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" s="55" t="s">
         <v>51</v>
       </c>
-      <c r="J6" s="56" t="s">
+      <c r="K6" s="55" t="s">
+        <v>70</v>
+      </c>
+      <c r="L6" s="57" t="s">
+        <v>75</v>
+      </c>
+      <c r="M6" s="67" t="s">
         <v>52</v>
-      </c>
-      <c r="K6" s="56" t="s">
-        <v>71</v>
-      </c>
-      <c r="L6" s="58" t="s">
-        <v>76</v>
-      </c>
-      <c r="M6" s="68" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:21" ht="101.25" x14ac:dyDescent="0.2">
       <c r="A7" s="11"/>
       <c r="B7" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="27" t="s">
         <v>1</v>
@@ -3195,33 +3307,33 @@
       <c r="D7" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E7" s="67" t="str">
+      <c r="E7" s="66" t="str">
         <f>IF(OR(AND(B7&lt;&gt;"Closed",C7="High",D7="High"),AND(B7&lt;&gt;"Closed",C7="High",D7="Medium"),AND(B7&lt;&gt;"Closed",C7="Medium",D7="High")),"Red",IF(OR(AND(B7&lt;&gt;"Closed",C7="High",D7="Low"),AND(B7&lt;&gt;"Closed",C7="Medium",D7="Medium"),AND(B7&lt;&gt;"Closed",C7="Low",D7="High")),"Yellow",IF(OR(AND(B7&lt;&gt;"Closed",C7="Medium",D7="Low"),AND(B7&lt;&gt;"Closed",C7="Low",D7="Low"),AND(B7&lt;&gt;"Closed",C7="Low",D7="Medium")),"Green",IF(B7="Closed","Closed",""))))</f>
         <v>Yellow</v>
       </c>
       <c r="F7" s="42" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G7" s="42" t="s">
+        <v>77</v>
+      </c>
+      <c r="H7" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="I7" s="42" t="s">
         <v>78</v>
       </c>
-      <c r="H7" s="41" t="s">
-        <v>77</v>
-      </c>
-      <c r="I7" s="42" t="s">
+      <c r="J7" s="42" t="s">
         <v>79</v>
       </c>
-      <c r="J7" s="42" t="s">
+      <c r="K7" s="75" t="s">
+        <v>69</v>
+      </c>
+      <c r="L7" s="42" t="s">
         <v>80</v>
       </c>
-      <c r="K7" s="76" t="s">
-        <v>70</v>
-      </c>
-      <c r="L7" s="42" t="s">
+      <c r="M7" s="64" t="s">
         <v>81</v>
-      </c>
-      <c r="M7" s="65" t="s">
-        <v>82</v>
       </c>
       <c r="O7" s="4" t="str">
         <f>IF(OR(AND(B7&lt;&gt;"Closed",C7="High",E7="High"), AND(B7&lt;&gt;"Closed",C7="High", E7="Medium"),AND(B7&lt;&gt;"Closed",C7="Medium",E7="High")),"Red",IF(OR(AND(B7&lt;&gt;"Closed",C7="High",E7="Low"), AND(B7&lt;&gt;"Closed",C7="Medium", E7="Medium"),AND(B7&lt;&gt;"Closed",C7="Low",E7="High")),"Yellow",IF(OR(AND(B7&lt;&gt;"Closed",C7="Medium",E7="Low"), AND(B7&lt;&gt;"Closed",C7="Low", E7="Low"),AND(B7&lt;&gt;"Closed",C7="Low",E7="Medium")),"Green","")))</f>
@@ -3231,7 +3343,7 @@
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A8" s="11"/>
       <c r="B8" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" s="27" t="s">
         <v>2</v>
@@ -3239,23 +3351,23 @@
       <c r="D8" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="67" t="str">
+      <c r="E8" s="66" t="str">
         <f>IF(OR(AND(B8&lt;&gt;"Closed",C8="High",D8="High"),AND(B8&lt;&gt;"Closed",C8="High",D8="Medium"),AND(B8&lt;&gt;"Closed",C8="Medium",D8="High")),"Red",IF(OR(AND(B8&lt;&gt;"Closed",C8="High",D8="Low"),AND(B8&lt;&gt;"Closed",C8="Medium",D8="Medium"),AND(B8&lt;&gt;"Closed",C8="Low",D8="High")),"Yellow",IF(OR(AND(B8&lt;&gt;"Closed",C8="Medium",D8="Low"),AND(B8&lt;&gt;"Closed",C8="Low",D8="Low"),AND(B8&lt;&gt;"Closed",C8="Low",D8="Medium")),"Green",IF(B8="Closed","Closed",""))))</f>
         <v>Yellow</v>
       </c>
       <c r="F8" s="42"/>
-      <c r="G8" s="66"/>
+      <c r="G8" s="65"/>
       <c r="H8" s="41"/>
-      <c r="I8" s="74"/>
-      <c r="J8" s="66"/>
-      <c r="K8" s="76"/>
-      <c r="L8" s="74"/>
+      <c r="I8" s="73"/>
+      <c r="J8" s="65"/>
+      <c r="K8" s="75"/>
+      <c r="L8" s="73"/>
       <c r="M8" s="43"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A9" s="11"/>
       <c r="B9" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="27" t="s">
         <v>3</v>
@@ -3263,25 +3375,25 @@
       <c r="D9" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E9" s="67" t="str">
+      <c r="E9" s="66" t="str">
         <f>IF(OR(AND(B9&lt;&gt;"Closed",C9="High",D9="High"),AND(B9&lt;&gt;"Closed",C9="High",D9="Medium"),AND(B9&lt;&gt;"Closed",C9="Medium",D9="High")),"Red",IF(OR(AND(B9&lt;&gt;"Closed",C9="High",D9="Low"),AND(B9&lt;&gt;"Closed",C9="Medium",D9="Medium"),AND(B9&lt;&gt;"Closed",C9="Low",D9="High")),"Yellow",IF(OR(AND(B9&lt;&gt;"Closed",C9="Medium",D9="Low"),AND(B9&lt;&gt;"Closed",C9="Low",D9="Low"),AND(B9&lt;&gt;"Closed",C9="Low",D9="Medium")),"Green",IF(B9="Closed","Closed",""))))</f>
         <v>Green</v>
       </c>
       <c r="F9" s="42"/>
-      <c r="G9" s="66"/>
+      <c r="G9" s="65"/>
       <c r="H9" s="41"/>
-      <c r="I9" s="74"/>
-      <c r="J9" s="66"/>
-      <c r="K9" s="76"/>
-      <c r="L9" s="74"/>
+      <c r="I9" s="73"/>
+      <c r="J9" s="65"/>
+      <c r="K9" s="75"/>
+      <c r="L9" s="73"/>
       <c r="M9" s="43"/>
     </row>
     <row r="10" spans="1:21" ht="78.75" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C10" s="27" t="s">
         <v>1</v>
@@ -3289,79 +3401,83 @@
       <c r="D10" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="67" t="str">
-        <f t="shared" ref="E10:E34" si="0">IF(OR(AND(B10&lt;&gt;"Closed",C10="High",D10="High"),AND(B10&lt;&gt;"Closed",C10="High",D10="Medium"),AND(B10&lt;&gt;"Closed",C10="Medium",D10="High")),"Red",IF(OR(AND(B10&lt;&gt;"Closed",C10="High",D10="Low"),AND(B10&lt;&gt;"Closed",C10="Medium",D10="Medium"),AND(B10&lt;&gt;"Closed",C10="Low",D10="High")),"Yellow",IF(OR(AND(B10&lt;&gt;"Closed",C10="Medium",D10="Low"),AND(B10&lt;&gt;"Closed",C10="Low",D10="Low"),AND(B10&lt;&gt;"Closed",C10="Low",D10="Medium")),"Green",IF(B10="Closed","Closed",""))))</f>
+      <c r="E10" s="66" t="str">
+        <f t="shared" ref="E10:E33" si="0">IF(OR(AND(B10&lt;&gt;"Closed",C10="High",D10="High"),AND(B10&lt;&gt;"Closed",C10="High",D10="Medium"),AND(B10&lt;&gt;"Closed",C10="Medium",D10="High")),"Red",IF(OR(AND(B10&lt;&gt;"Closed",C10="High",D10="Low"),AND(B10&lt;&gt;"Closed",C10="Medium",D10="Medium"),AND(B10&lt;&gt;"Closed",C10="Low",D10="High")),"Yellow",IF(OR(AND(B10&lt;&gt;"Closed",C10="Medium",D10="Low"),AND(B10&lt;&gt;"Closed",C10="Low",D10="Low"),AND(B10&lt;&gt;"Closed",C10="Low",D10="Medium")),"Green",IF(B10="Closed","Closed",""))))</f>
         <v>Yellow</v>
       </c>
-      <c r="F10" s="79" t="s">
+      <c r="F10" s="78" t="s">
+        <v>86</v>
+      </c>
+      <c r="G10" s="79" t="s">
         <v>87</v>
       </c>
-      <c r="G10" s="80" t="s">
+      <c r="H10" s="41" t="s">
+        <v>97</v>
+      </c>
+      <c r="I10" s="80" t="s">
         <v>88</v>
       </c>
-      <c r="H10" s="41" t="s">
-        <v>98</v>
-      </c>
-      <c r="I10" s="81" t="s">
+      <c r="J10" s="79" t="s">
         <v>89</v>
       </c>
-      <c r="J10" s="80" t="s">
+      <c r="K10" s="75" t="s">
+        <v>69</v>
+      </c>
+      <c r="L10" s="82" t="s">
         <v>90</v>
       </c>
-      <c r="K10" s="76" t="s">
-        <v>70</v>
-      </c>
-      <c r="L10" s="83" t="s">
+      <c r="M10" s="83" t="s">
         <v>91</v>
       </c>
-      <c r="M10" s="84" t="s">
-        <v>92</v>
-      </c>
     </row>
     <row r="11" spans="1:21" ht="101.25" x14ac:dyDescent="0.2">
-      <c r="A11" s="11"/>
+      <c r="A11" s="11" t="s">
+        <v>170</v>
+      </c>
       <c r="B11" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="D11" s="64" t="s">
+      <c r="D11" s="63" t="s">
         <v>3</v>
       </c>
-      <c r="E11" s="67" t="str">
+      <c r="E11" s="66" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
       </c>
       <c r="F11" s="44" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G11" s="41" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H11" s="41" t="s">
-        <v>98</v>
-      </c>
-      <c r="I11" s="81" t="s">
+        <v>97</v>
+      </c>
+      <c r="I11" s="80" t="s">
+        <v>107</v>
+      </c>
+      <c r="J11" s="79" t="s">
         <v>108</v>
       </c>
-      <c r="J11" s="80" t="s">
+      <c r="K11" s="75" t="s">
         <v>109</v>
       </c>
-      <c r="K11" s="76" t="s">
+      <c r="L11" s="84" t="s">
         <v>110</v>
       </c>
-      <c r="L11" s="85" t="s">
+      <c r="M11" s="46" t="s">
         <v>111</v>
       </c>
-      <c r="M11" s="46" t="s">
-        <v>112</v>
-      </c>
     </row>
     <row r="12" spans="1:21" ht="112.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="12"/>
+      <c r="A12" s="11" t="s">
+        <v>171</v>
+      </c>
       <c r="B12" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12" s="27" t="s">
         <v>1</v>
@@ -3369,39 +3485,41 @@
       <c r="D12" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E12" s="67" t="str">
+      <c r="E12" s="66" t="str">
         <f t="shared" si="0"/>
         <v>Yellow</v>
       </c>
       <c r="F12" s="45" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G12" s="41" t="s">
+        <v>112</v>
+      </c>
+      <c r="H12" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="H12" s="41" t="s">
+      <c r="I12" s="80" t="s">
         <v>114</v>
       </c>
-      <c r="I12" s="81" t="s">
+      <c r="J12" s="79" t="s">
         <v>115</v>
       </c>
-      <c r="J12" s="80" t="s">
-        <v>116</v>
-      </c>
-      <c r="K12" s="76" t="s">
-        <v>70</v>
-      </c>
-      <c r="L12" s="82" t="s">
-        <v>117</v>
+      <c r="K12" s="75" t="s">
+        <v>69</v>
+      </c>
+      <c r="L12" s="81" t="s">
+        <v>185</v>
       </c>
       <c r="M12" s="47" t="s">
-        <v>118</v>
+        <v>186</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="146.25" x14ac:dyDescent="0.2">
-      <c r="A13" s="12"/>
+      <c r="A13" s="11" t="s">
+        <v>172</v>
+      </c>
       <c r="B13" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C13" s="27" t="s">
         <v>2</v>
@@ -3409,39 +3527,41 @@
       <c r="D13" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E13" s="67" t="str">
+      <c r="E13" s="66" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
       </c>
       <c r="F13" s="45" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G13" s="41" t="s">
+        <v>116</v>
+      </c>
+      <c r="H13" s="41" t="s">
+        <v>117</v>
+      </c>
+      <c r="I13" s="80" t="s">
+        <v>118</v>
+      </c>
+      <c r="J13" s="79" t="s">
         <v>119</v>
       </c>
-      <c r="H13" s="41" t="s">
-        <v>120</v>
-      </c>
-      <c r="I13" s="81" t="s">
-        <v>121</v>
-      </c>
-      <c r="J13" s="80" t="s">
-        <v>122</v>
-      </c>
-      <c r="K13" s="76" t="s">
-        <v>70</v>
-      </c>
-      <c r="L13" s="82" t="s">
-        <v>123</v>
+      <c r="K13" s="75" t="s">
+        <v>69</v>
+      </c>
+      <c r="L13" s="81" t="s">
+        <v>183</v>
       </c>
       <c r="M13" s="47" t="s">
-        <v>124</v>
+        <v>184</v>
       </c>
     </row>
     <row r="14" spans="1:21" ht="123.75" x14ac:dyDescent="0.2">
-      <c r="A14" s="12"/>
+      <c r="A14" s="11" t="s">
+        <v>173</v>
+      </c>
       <c r="B14" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C14" s="27" t="s">
         <v>1</v>
@@ -3449,39 +3569,41 @@
       <c r="D14" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E14" s="67" t="str">
+      <c r="E14" s="66" t="str">
         <f t="shared" si="0"/>
         <v>Yellow</v>
       </c>
       <c r="F14" s="45" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G14" s="41" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="H14" s="41" t="s">
-        <v>120</v>
-      </c>
-      <c r="I14" s="81" t="s">
-        <v>126</v>
-      </c>
-      <c r="J14" s="80" t="s">
-        <v>127</v>
-      </c>
-      <c r="K14" s="76" t="s">
-        <v>70</v>
-      </c>
-      <c r="L14" s="82" t="s">
-        <v>128</v>
+        <v>117</v>
+      </c>
+      <c r="I14" s="80" t="s">
+        <v>121</v>
+      </c>
+      <c r="J14" s="79" t="s">
+        <v>122</v>
+      </c>
+      <c r="K14" s="75" t="s">
+        <v>69</v>
+      </c>
+      <c r="L14" s="81" t="s">
+        <v>123</v>
       </c>
       <c r="M14" s="47" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="146.25" x14ac:dyDescent="0.2">
-      <c r="A15" s="12"/>
+      <c r="A15" s="11" t="s">
+        <v>174</v>
+      </c>
       <c r="B15" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C15" s="27" t="s">
         <v>1</v>
@@ -3489,39 +3611,41 @@
       <c r="D15" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E15" s="67" t="str">
+      <c r="E15" s="66" t="str">
         <f t="shared" si="0"/>
         <v>Yellow</v>
       </c>
       <c r="F15" s="45" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G15" s="41" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="H15" s="41" t="s">
-        <v>138</v>
-      </c>
-      <c r="I15" s="81" t="s">
-        <v>142</v>
-      </c>
-      <c r="J15" s="80" t="s">
-        <v>151</v>
-      </c>
-      <c r="K15" s="76" t="s">
-        <v>70</v>
-      </c>
-      <c r="L15" s="82" t="s">
-        <v>159</v>
+        <v>133</v>
+      </c>
+      <c r="I15" s="80" t="s">
+        <v>137</v>
+      </c>
+      <c r="J15" s="79" t="s">
+        <v>146</v>
+      </c>
+      <c r="K15" s="75" t="s">
+        <v>69</v>
+      </c>
+      <c r="L15" s="81" t="s">
+        <v>154</v>
       </c>
       <c r="M15" s="47" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="157.5" x14ac:dyDescent="0.2">
-      <c r="A16" s="12"/>
+      <c r="A16" s="11" t="s">
+        <v>175</v>
+      </c>
       <c r="B16" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C16" s="27" t="s">
         <v>1</v>
@@ -3529,39 +3653,41 @@
       <c r="D16" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E16" s="67" t="str">
+      <c r="E16" s="66" t="str">
         <f t="shared" si="0"/>
         <v>Yellow</v>
       </c>
       <c r="F16" s="45" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G16" s="41" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H16" s="41" t="s">
-        <v>139</v>
-      </c>
-      <c r="I16" s="81" t="s">
-        <v>143</v>
-      </c>
-      <c r="J16" s="80" t="s">
-        <v>150</v>
-      </c>
-      <c r="K16" s="76" t="s">
-        <v>70</v>
-      </c>
-      <c r="L16" s="82" t="s">
-        <v>160</v>
+        <v>134</v>
+      </c>
+      <c r="I16" s="80" t="s">
+        <v>138</v>
+      </c>
+      <c r="J16" s="79" t="s">
+        <v>145</v>
+      </c>
+      <c r="K16" s="75" t="s">
+        <v>69</v>
+      </c>
+      <c r="L16" s="81" t="s">
+        <v>155</v>
       </c>
       <c r="M16" s="47" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="123.75" x14ac:dyDescent="0.2">
-      <c r="A17" s="12"/>
+      <c r="A17" s="11" t="s">
+        <v>176</v>
+      </c>
       <c r="B17" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C17" s="27" t="s">
         <v>1</v>
@@ -3569,39 +3695,41 @@
       <c r="D17" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E17" s="67" t="str">
+      <c r="E17" s="66" t="str">
         <f t="shared" si="0"/>
         <v>Yellow</v>
       </c>
       <c r="F17" s="45" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G17" s="41" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="H17" s="41" t="s">
-        <v>46</v>
-      </c>
-      <c r="I17" s="81" t="s">
-        <v>144</v>
-      </c>
-      <c r="J17" s="80" t="s">
-        <v>152</v>
-      </c>
-      <c r="K17" s="76" t="s">
-        <v>70</v>
-      </c>
-      <c r="L17" s="82" t="s">
-        <v>162</v>
+        <v>45</v>
+      </c>
+      <c r="I17" s="80" t="s">
+        <v>139</v>
+      </c>
+      <c r="J17" s="79" t="s">
+        <v>147</v>
+      </c>
+      <c r="K17" s="75" t="s">
+        <v>69</v>
+      </c>
+      <c r="L17" s="81" t="s">
+        <v>157</v>
       </c>
       <c r="M17" s="47" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="18" spans="1:13" ht="78.75" x14ac:dyDescent="0.2">
-      <c r="A18" s="12"/>
+      <c r="A18" s="11" t="s">
+        <v>177</v>
+      </c>
       <c r="B18" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C18" s="27" t="s">
         <v>2</v>
@@ -3609,39 +3737,41 @@
       <c r="D18" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E18" s="67" t="str">
+      <c r="E18" s="66" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
       </c>
       <c r="F18" s="45" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G18" s="41" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="H18" s="41" t="s">
-        <v>139</v>
-      </c>
-      <c r="I18" s="81" t="s">
-        <v>145</v>
-      </c>
-      <c r="J18" s="80" t="s">
-        <v>153</v>
-      </c>
-      <c r="K18" s="76" t="s">
-        <v>70</v>
-      </c>
-      <c r="L18" s="82" t="s">
-        <v>164</v>
+        <v>134</v>
+      </c>
+      <c r="I18" s="80" t="s">
+        <v>140</v>
+      </c>
+      <c r="J18" s="79" t="s">
+        <v>148</v>
+      </c>
+      <c r="K18" s="75" t="s">
+        <v>69</v>
+      </c>
+      <c r="L18" s="81" t="s">
+        <v>159</v>
       </c>
       <c r="M18" s="47" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="19" spans="1:13" ht="90" x14ac:dyDescent="0.2">
-      <c r="A19" s="12"/>
+      <c r="A19" s="11" t="s">
+        <v>178</v>
+      </c>
       <c r="B19" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C19" s="27" t="s">
         <v>2</v>
@@ -3649,39 +3779,41 @@
       <c r="D19" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E19" s="67" t="str">
+      <c r="E19" s="66" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
       </c>
       <c r="F19" s="45" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G19" s="41" t="s">
+        <v>129</v>
+      </c>
+      <c r="H19" s="41" t="s">
         <v>134</v>
       </c>
-      <c r="H19" s="41" t="s">
-        <v>139</v>
-      </c>
-      <c r="I19" s="81" t="s">
-        <v>146</v>
-      </c>
-      <c r="J19" s="80" t="s">
-        <v>154</v>
-      </c>
-      <c r="K19" s="76" t="s">
-        <v>70</v>
-      </c>
-      <c r="L19" s="82" t="s">
-        <v>164</v>
+      <c r="I19" s="80" t="s">
+        <v>141</v>
+      </c>
+      <c r="J19" s="79" t="s">
+        <v>149</v>
+      </c>
+      <c r="K19" s="75" t="s">
+        <v>69</v>
+      </c>
+      <c r="L19" s="81" t="s">
+        <v>159</v>
       </c>
       <c r="M19" s="47" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="20" spans="1:13" ht="112.5" x14ac:dyDescent="0.2">
-      <c r="A20" s="12"/>
+      <c r="A20" s="11" t="s">
+        <v>179</v>
+      </c>
       <c r="B20" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C20" s="27" t="s">
         <v>2</v>
@@ -3689,39 +3821,41 @@
       <c r="D20" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E20" s="67" t="str">
+      <c r="E20" s="66" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
       </c>
       <c r="F20" s="45" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G20" s="41" t="s">
+        <v>130</v>
+      </c>
+      <c r="H20" s="41" t="s">
         <v>135</v>
       </c>
-      <c r="H20" s="41" t="s">
-        <v>140</v>
-      </c>
-      <c r="I20" s="81" t="s">
-        <v>147</v>
-      </c>
-      <c r="J20" s="80" t="s">
-        <v>155</v>
-      </c>
-      <c r="K20" s="76" t="s">
-        <v>70</v>
-      </c>
-      <c r="L20" s="82" t="s">
-        <v>166</v>
+      <c r="I20" s="80" t="s">
+        <v>142</v>
+      </c>
+      <c r="J20" s="79" t="s">
+        <v>150</v>
+      </c>
+      <c r="K20" s="75" t="s">
+        <v>69</v>
+      </c>
+      <c r="L20" s="81" t="s">
+        <v>161</v>
       </c>
       <c r="M20" s="47" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="21" spans="1:13" ht="90" x14ac:dyDescent="0.2">
-      <c r="A21" s="12"/>
+      <c r="A21" s="11" t="s">
+        <v>180</v>
+      </c>
       <c r="B21" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C21" s="27" t="s">
         <v>2</v>
@@ -3729,39 +3863,41 @@
       <c r="D21" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E21" s="67" t="str">
+      <c r="E21" s="66" t="str">
         <f t="shared" si="0"/>
         <v>Green</v>
       </c>
       <c r="F21" s="45" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G21" s="41" t="s">
+        <v>131</v>
+      </c>
+      <c r="H21" s="41" t="s">
         <v>136</v>
       </c>
-      <c r="H21" s="41" t="s">
-        <v>141</v>
-      </c>
-      <c r="I21" s="81" t="s">
-        <v>148</v>
-      </c>
-      <c r="J21" s="80" t="s">
-        <v>156</v>
-      </c>
-      <c r="K21" s="76" t="s">
-        <v>70</v>
-      </c>
-      <c r="L21" s="82" t="s">
-        <v>168</v>
+      <c r="I21" s="80" t="s">
+        <v>143</v>
+      </c>
+      <c r="J21" s="79" t="s">
+        <v>151</v>
+      </c>
+      <c r="K21" s="75" t="s">
+        <v>69</v>
+      </c>
+      <c r="L21" s="81" t="s">
+        <v>163</v>
       </c>
       <c r="M21" s="47" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="22" spans="1:13" ht="123.75" x14ac:dyDescent="0.2">
-      <c r="A22" s="12"/>
+      <c r="A22" s="11" t="s">
+        <v>181</v>
+      </c>
       <c r="B22" s="14" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C22" s="27" t="s">
         <v>1</v>
@@ -3769,69 +3905,93 @@
       <c r="D22" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="E22" s="67" t="str">
+      <c r="E22" s="66" t="str">
         <f t="shared" si="0"/>
         <v>Yellow</v>
       </c>
       <c r="F22" s="45" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G22" s="41" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="H22" s="41" t="s">
-        <v>141</v>
-      </c>
-      <c r="I22" s="81" t="s">
-        <v>149</v>
-      </c>
-      <c r="J22" s="80" t="s">
-        <v>157</v>
-      </c>
-      <c r="K22" s="76" t="s">
-        <v>70</v>
-      </c>
-      <c r="L22" s="82" t="s">
-        <v>170</v>
+        <v>136</v>
+      </c>
+      <c r="I22" s="80" t="s">
+        <v>144</v>
+      </c>
+      <c r="J22" s="79" t="s">
+        <v>152</v>
+      </c>
+      <c r="K22" s="75" t="s">
+        <v>69</v>
+      </c>
+      <c r="L22" s="81" t="s">
+        <v>165</v>
       </c>
       <c r="M22" s="47" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A23" s="12"/>
-      <c r="B23" s="14"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="67" t="str">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A23" s="12" t="s">
+        <v>182</v>
+      </c>
+      <c r="B23" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" s="27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E23" s="66" t="str">
         <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="F23" s="45"/>
-      <c r="G23" s="41"/>
-      <c r="H23" s="41"/>
-      <c r="I23" s="74"/>
-      <c r="J23" s="66"/>
-      <c r="K23" s="76"/>
-      <c r="L23" s="82"/>
-      <c r="M23" s="47"/>
+        <v>Green</v>
+      </c>
+      <c r="F23" s="91" t="s">
+        <v>187</v>
+      </c>
+      <c r="G23" s="92" t="s">
+        <v>188</v>
+      </c>
+      <c r="H23" s="92" t="s">
+        <v>45</v>
+      </c>
+      <c r="I23" s="93" t="s">
+        <v>189</v>
+      </c>
+      <c r="J23" s="94" t="s">
+        <v>190</v>
+      </c>
+      <c r="K23" s="95" t="s">
+        <v>69</v>
+      </c>
+      <c r="L23" s="96" t="s">
+        <v>192</v>
+      </c>
+      <c r="M23" s="97" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" s="12"/>
       <c r="B24" s="14"/>
       <c r="C24" s="27"/>
       <c r="D24" s="27"/>
-      <c r="E24" s="67" t="str">
+      <c r="E24" s="66" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="F24" s="45"/>
       <c r="G24" s="41"/>
       <c r="H24" s="41"/>
-      <c r="I24" s="74"/>
-      <c r="J24" s="66"/>
-      <c r="K24" s="76"/>
-      <c r="L24" s="82"/>
+      <c r="I24" s="73"/>
+      <c r="J24" s="65"/>
+      <c r="K24" s="75"/>
+      <c r="L24" s="81"/>
       <c r="M24" s="47"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
@@ -3839,17 +3999,17 @@
       <c r="B25" s="14"/>
       <c r="C25" s="27"/>
       <c r="D25" s="27"/>
-      <c r="E25" s="67" t="str">
+      <c r="E25" s="66" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="F25" s="45"/>
       <c r="G25" s="41"/>
       <c r="H25" s="41"/>
-      <c r="I25" s="74"/>
-      <c r="J25" s="66"/>
-      <c r="K25" s="76"/>
-      <c r="L25" s="82"/>
+      <c r="I25" s="73"/>
+      <c r="J25" s="65"/>
+      <c r="K25" s="75"/>
+      <c r="L25" s="81"/>
       <c r="M25" s="47"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.2">
@@ -3857,17 +4017,17 @@
       <c r="B26" s="14"/>
       <c r="C26" s="27"/>
       <c r="D26" s="27"/>
-      <c r="E26" s="67" t="str">
+      <c r="E26" s="66" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="F26" s="45"/>
       <c r="G26" s="41"/>
       <c r="H26" s="41"/>
-      <c r="I26" s="74"/>
-      <c r="J26" s="66"/>
-      <c r="K26" s="76"/>
-      <c r="L26" s="82"/>
+      <c r="I26" s="73"/>
+      <c r="J26" s="65"/>
+      <c r="K26" s="75"/>
+      <c r="L26" s="81"/>
       <c r="M26" s="47"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.2">
@@ -3875,17 +4035,17 @@
       <c r="B27" s="14"/>
       <c r="C27" s="27"/>
       <c r="D27" s="27"/>
-      <c r="E27" s="67" t="str">
+      <c r="E27" s="66" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="F27" s="45"/>
       <c r="G27" s="41"/>
       <c r="H27" s="41"/>
-      <c r="I27" s="74"/>
-      <c r="J27" s="66"/>
-      <c r="K27" s="76"/>
-      <c r="L27" s="82"/>
+      <c r="I27" s="73"/>
+      <c r="J27" s="65"/>
+      <c r="K27" s="75"/>
+      <c r="L27" s="81"/>
       <c r="M27" s="47"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.2">
@@ -3893,17 +4053,17 @@
       <c r="B28" s="14"/>
       <c r="C28" s="27"/>
       <c r="D28" s="27"/>
-      <c r="E28" s="67" t="str">
+      <c r="E28" s="66" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="F28" s="45"/>
       <c r="G28" s="41"/>
       <c r="H28" s="41"/>
-      <c r="I28" s="74"/>
-      <c r="J28" s="66"/>
-      <c r="K28" s="76"/>
-      <c r="L28" s="82"/>
+      <c r="I28" s="73"/>
+      <c r="J28" s="65"/>
+      <c r="K28" s="75"/>
+      <c r="L28" s="81"/>
       <c r="M28" s="47"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.2">
@@ -3911,17 +4071,17 @@
       <c r="B29" s="14"/>
       <c r="C29" s="27"/>
       <c r="D29" s="27"/>
-      <c r="E29" s="67" t="str">
+      <c r="E29" s="66" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="F29" s="45"/>
       <c r="G29" s="41"/>
       <c r="H29" s="41"/>
-      <c r="I29" s="74"/>
-      <c r="J29" s="66"/>
-      <c r="K29" s="76"/>
-      <c r="L29" s="82"/>
+      <c r="I29" s="73"/>
+      <c r="J29" s="65"/>
+      <c r="K29" s="75"/>
+      <c r="L29" s="81"/>
       <c r="M29" s="47"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.2">
@@ -3929,17 +4089,17 @@
       <c r="B30" s="14"/>
       <c r="C30" s="27"/>
       <c r="D30" s="27"/>
-      <c r="E30" s="67" t="str">
+      <c r="E30" s="66" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="F30" s="45"/>
       <c r="G30" s="41"/>
       <c r="H30" s="41"/>
-      <c r="I30" s="74"/>
-      <c r="J30" s="66"/>
-      <c r="K30" s="76"/>
-      <c r="L30" s="82"/>
+      <c r="I30" s="73"/>
+      <c r="J30" s="65"/>
+      <c r="K30" s="75"/>
+      <c r="L30" s="81"/>
       <c r="M30" s="47"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.2">
@@ -3947,17 +4107,17 @@
       <c r="B31" s="14"/>
       <c r="C31" s="27"/>
       <c r="D31" s="27"/>
-      <c r="E31" s="67" t="str">
+      <c r="E31" s="66" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="F31" s="45"/>
       <c r="G31" s="41"/>
       <c r="H31" s="41"/>
-      <c r="I31" s="74"/>
-      <c r="J31" s="66"/>
-      <c r="K31" s="76"/>
-      <c r="L31" s="82"/>
+      <c r="I31" s="73"/>
+      <c r="J31" s="65"/>
+      <c r="K31" s="75"/>
+      <c r="L31" s="81"/>
       <c r="M31" s="47"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.2">
@@ -3965,59 +4125,41 @@
       <c r="B32" s="14"/>
       <c r="C32" s="27"/>
       <c r="D32" s="27"/>
-      <c r="E32" s="67" t="str">
+      <c r="E32" s="66" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="F32" s="45"/>
       <c r="G32" s="41"/>
       <c r="H32" s="41"/>
-      <c r="I32" s="74"/>
-      <c r="J32" s="66"/>
-      <c r="K32" s="76"/>
-      <c r="L32" s="82"/>
+      <c r="I32" s="73"/>
+      <c r="J32" s="65"/>
+      <c r="K32" s="75"/>
+      <c r="L32" s="81"/>
       <c r="M32" s="47"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A33" s="12"/>
-      <c r="B33" s="14"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="67" t="str">
+    <row r="33" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="13"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="61"/>
+      <c r="D33" s="61"/>
+      <c r="E33" s="15" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="F33" s="45"/>
-      <c r="G33" s="41"/>
-      <c r="H33" s="41"/>
-      <c r="I33" s="74"/>
-      <c r="J33" s="66"/>
-      <c r="K33" s="76"/>
-      <c r="L33" s="82"/>
-      <c r="M33" s="47"/>
-    </row>
-    <row r="34" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="13"/>
-      <c r="B34" s="15"/>
-      <c r="C34" s="62"/>
-      <c r="D34" s="62"/>
-      <c r="E34" s="15" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="F34" s="48"/>
-      <c r="G34" s="63"/>
-      <c r="H34" s="63"/>
-      <c r="I34" s="72"/>
-      <c r="J34" s="73"/>
-      <c r="K34" s="75"/>
-      <c r="L34" s="86"/>
-      <c r="M34" s="49"/>
+      <c r="F33" s="48"/>
+      <c r="G33" s="62"/>
+      <c r="H33" s="62"/>
+      <c r="I33" s="71"/>
+      <c r="J33" s="72"/>
+      <c r="K33" s="74"/>
+      <c r="L33" s="85"/>
+      <c r="M33" s="49"/>
     </row>
   </sheetData>
-  <autoFilter ref="B6:D6" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="B6:D6"/>
   <phoneticPr fontId="3" type="noConversion"/>
-  <conditionalFormatting sqref="C35:E65535 C1:E1 B6:C6 B7:B34">
+  <conditionalFormatting sqref="C34:E65534 C1:E1 B6:C6 B7:B33">
     <cfRule type="cellIs" dxfId="10" priority="1" stopIfTrue="1" operator="equal">
       <formula>"Critical"</formula>
     </cfRule>
@@ -4028,7 +4170,7 @@
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L10:L34">
+  <conditionalFormatting sqref="L10:L33">
     <cfRule type="cellIs" dxfId="7" priority="4" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
@@ -4036,7 +4178,7 @@
       <formula>"Medium"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E7:E34">
+  <conditionalFormatting sqref="E7:E33">
     <cfRule type="cellIs" dxfId="5" priority="6" stopIfTrue="1" operator="equal">
       <formula>"Red"</formula>
     </cfRule>
@@ -4047,7 +4189,7 @@
       <formula>"Green"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C7:D34">
+  <conditionalFormatting sqref="C7:D33">
     <cfRule type="cellIs" dxfId="2" priority="9" stopIfTrue="1" operator="equal">
       <formula>"High"</formula>
     </cfRule>
@@ -4059,16 +4201,16 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7:D34" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C7:D33">
       <formula1>"High,Medium,Low"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7:H34" xr:uid="{00000000-0002-0000-0100-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H7:H33">
       <formula1>Risk_Area</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:B34" xr:uid="{00000000-0002-0000-0100-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:B33">
       <formula1>"Open,Closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K7:K34" xr:uid="{00000000-0002-0000-0100-000003000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K7:K33">
       <formula1>"Acceptance,Avoidance,Contingency,Mitigation,Transfer"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4082,7 +4224,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4095,103 +4237,103 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="58" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="59" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="60" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="59" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="60" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="59" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="60" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" s="59" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="60" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="59" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="60" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="59" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="60" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="59" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="60" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="59" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="60" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="59" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="60" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="59" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="60" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A12" s="59" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="60" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A13" s="59" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="60" t="s">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="59" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="60" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A15" s="59" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="60" t="s">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="59" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="60" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="59" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="60" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="59" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="60" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="59" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="60" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="59" t="s">
         <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="60" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>